<commit_message>
updated checklist, backlog and review docs
</commit_message>
<xml_diff>
--- a/Documents/Deliverable drafts_&_templates/Deliverable 2/SixGuys_Deliverable_2_ProductBackLog_2.xlsx
+++ b/Documents/Deliverable drafts_&_templates/Deliverable 2/SixGuys_Deliverable_2_ProductBackLog_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Project-Burger\Documents\Deliverable drafts_&amp;_templates\Deliverable 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51BD8D6-C0AB-4F70-BC7B-FC24B39EA584}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF90D9E-1712-4768-8575-2434EF9F07DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21900" windowHeight="15180" xr2:uid="{BB07E46C-EBB9-4E59-B503-407F69F25581}"/>
   </bookViews>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1140,9 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="5">
+        <v>2</v>
+      </c>
       <c r="B7" s="17" t="s">
         <v>60</v>
       </c>

</xml_diff>